<commit_message>
Fixed the bug of access to folders which should be private; Add products of minnetonka, jawbone and brand nike
</commit_message>
<xml_diff>
--- a/Logpie.xlsx
+++ b/Logpie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="护肤品1000" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="母婴4000" sheetId="3" r:id="rId4"/>
     <sheet name="保健品5000" sheetId="5" r:id="rId5"/>
     <sheet name="服饰6000" sheetId="6" r:id="rId6"/>
+    <sheet name="运动类7000" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="360">
   <si>
     <t>Fresh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1341,6 +1342,121 @@
   </si>
   <si>
     <t>女士柔软内绒外套-玫红</t>
+  </si>
+  <si>
+    <t>5/5.5/6/6.5/7/7.5/8</t>
+  </si>
+  <si>
+    <t>5/5.5/6/6.5/7/7.5/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5/5.5/6/6.5/7/7.5/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帆布平底鞋_米色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帆布平底鞋_浅蓝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minnetonka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HelloKitty系列平底鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麂皮绒平底鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>步行平底鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皮革鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平底鞋_深棕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流苏平底鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>软底平底鞋(宽版)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>克里斯内绒鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脚踝单靴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内绒流苏靴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>船鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jawbone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动手环-黑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动手环-红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动手环-蓝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运动手环-银</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2代运动手环-黑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2代运动手环-蓝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2代运动手环-红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2代运动手环-粉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2代运动手环-橙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/M/L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/M/L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1356,7 +1472,7 @@
     <numFmt numFmtId="178" formatCode="_ [$￥-804]* #,##0.00_ ;_ [$￥-804]* \-#,##0.00_ ;_ [$￥-804]* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1432,6 +1548,11 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Extra Bold"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1633,7 +1754,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1693,8 +1814,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2032,28 +2171,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="39" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2097,8 +2215,38 @@
     <xf numFmtId="179" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="77">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -2144,6 +2292,24 @@
     <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -2497,9 +2663,9 @@
   <dimension ref="B1:Y93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>
@@ -2539,14 +2705,14 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="131"/>
+      <c r="H1" s="131" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="114"/>
+      <c r="I1" s="131"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -2559,10 +2725,10 @@
       <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="114" t="s">
+      <c r="N1" s="131" t="s">
         <v>256</v>
       </c>
-      <c r="O1" s="114"/>
+      <c r="O1" s="131"/>
       <c r="P1" s="88" t="s">
         <v>273</v>
       </c>
@@ -3142,7 +3308,7 @@
         <f t="shared" ref="L12:L28" si="9">K12-I12</f>
         <v>40.977637500000014</v>
       </c>
-      <c r="M12" s="118" t="s">
+      <c r="M12" s="135" t="s">
         <v>38</v>
       </c>
       <c r="N12" s="13">
@@ -3203,7 +3369,7 @@
         <f t="shared" si="9"/>
         <v>46.621137500000032</v>
       </c>
-      <c r="M13" s="119"/>
+      <c r="M13" s="136"/>
       <c r="N13" s="13"/>
       <c r="O13" s="11" t="s">
         <v>80</v>
@@ -3260,7 +3426,7 @@
         <f t="shared" si="9"/>
         <v>37.541987500000005</v>
       </c>
-      <c r="M14" s="119"/>
+      <c r="M14" s="136"/>
       <c r="N14" s="13">
         <v>300</v>
       </c>
@@ -3319,7 +3485,7 @@
         <f t="shared" si="9"/>
         <v>43.262225000000058</v>
       </c>
-      <c r="M15" s="119"/>
+      <c r="M15" s="136"/>
       <c r="N15" s="13"/>
       <c r="O15" s="11" t="s">
         <v>82</v>
@@ -3376,7 +3542,7 @@
         <f t="shared" si="9"/>
         <v>44.490025000000003</v>
       </c>
-      <c r="M16" s="119"/>
+      <c r="M16" s="136"/>
       <c r="N16" s="13">
         <v>280</v>
       </c>
@@ -3435,7 +3601,7 @@
         <f t="shared" si="9"/>
         <v>37.925675000000012</v>
       </c>
-      <c r="M17" s="119"/>
+      <c r="M17" s="136"/>
       <c r="N17" s="13"/>
       <c r="O17" s="11"/>
       <c r="P17" s="12">
@@ -3490,7 +3656,7 @@
         <f t="shared" si="9"/>
         <v>43.87612500000003</v>
       </c>
-      <c r="M18" s="119"/>
+      <c r="M18" s="136"/>
       <c r="N18" s="13">
         <v>330</v>
       </c>
@@ -3549,7 +3715,7 @@
         <f t="shared" si="9"/>
         <v>66.467662500000017</v>
       </c>
-      <c r="M19" s="119"/>
+      <c r="M19" s="136"/>
       <c r="N19" s="13">
         <v>520</v>
       </c>
@@ -3608,7 +3774,7 @@
         <f t="shared" si="9"/>
         <v>68.445300000000032</v>
       </c>
-      <c r="M20" s="119"/>
+      <c r="M20" s="136"/>
       <c r="N20" s="13"/>
       <c r="O20" s="11">
         <v>509</v>
@@ -3665,7 +3831,7 @@
         <f t="shared" si="9"/>
         <v>49.980050000000006</v>
       </c>
-      <c r="M21" s="119"/>
+      <c r="M21" s="136"/>
       <c r="N21" s="13">
         <v>450</v>
       </c>
@@ -3724,7 +3890,7 @@
         <f t="shared" si="9"/>
         <v>68.75225000000006</v>
       </c>
-      <c r="M22" s="119"/>
+      <c r="M22" s="136"/>
       <c r="N22" s="13"/>
       <c r="O22" s="11"/>
       <c r="P22" s="12">
@@ -3779,7 +3945,7 @@
         <f t="shared" si="9"/>
         <v>21.975225000000002</v>
       </c>
-      <c r="M23" s="119"/>
+      <c r="M23" s="136"/>
       <c r="N23" s="13"/>
       <c r="O23" s="11">
         <v>65</v>
@@ -3836,7 +4002,7 @@
         <f t="shared" si="9"/>
         <v>28.079149999999998</v>
       </c>
-      <c r="M24" s="119"/>
+      <c r="M24" s="136"/>
       <c r="N24" s="13">
         <v>180</v>
       </c>
@@ -3895,7 +4061,7 @@
         <f t="shared" si="9"/>
         <v>50.900900000000007</v>
       </c>
-      <c r="M25" s="119"/>
+      <c r="M25" s="136"/>
       <c r="N25" s="13">
         <v>340</v>
       </c>
@@ -3954,7 +4120,7 @@
         <f t="shared" si="9"/>
         <v>21.975225000000002</v>
       </c>
-      <c r="M26" s="119"/>
+      <c r="M26" s="136"/>
       <c r="N26" s="13"/>
       <c r="O26" s="11"/>
       <c r="P26" s="12">
@@ -4009,7 +4175,7 @@
         <f t="shared" si="9"/>
         <v>31.361325000000008</v>
       </c>
-      <c r="M27" s="119"/>
+      <c r="M27" s="136"/>
       <c r="N27" s="13">
         <v>220</v>
       </c>
@@ -4068,7 +4234,7 @@
         <f t="shared" si="9"/>
         <v>57.465249999999997</v>
       </c>
-      <c r="M28" s="120"/>
+      <c r="M28" s="137"/>
       <c r="N28" s="13">
         <v>360</v>
       </c>
@@ -4150,7 +4316,7 @@
         <f t="shared" ref="L30:L36" si="14">K30-I30</f>
         <v>72.494849999999985</v>
       </c>
-      <c r="M30" s="117" t="s">
+      <c r="M30" s="134" t="s">
         <v>46</v>
       </c>
       <c r="N30" s="13">
@@ -4206,7 +4372,7 @@
         <f t="shared" si="14"/>
         <v>100.96010000000001</v>
       </c>
-      <c r="M31" s="117"/>
+      <c r="M31" s="134"/>
       <c r="N31" s="13">
         <v>950</v>
       </c>
@@ -4260,7 +4426,7 @@
         <f t="shared" si="14"/>
         <v>59.366150000000005</v>
       </c>
-      <c r="M32" s="117"/>
+      <c r="M32" s="134"/>
       <c r="N32" s="13">
         <v>560</v>
       </c>
@@ -4314,7 +4480,7 @@
         <f t="shared" si="14"/>
         <v>73.341375000000028</v>
       </c>
-      <c r="M33" s="117"/>
+      <c r="M33" s="134"/>
       <c r="N33" s="13">
         <v>650</v>
       </c>
@@ -4368,7 +4534,7 @@
         <f t="shared" si="14"/>
         <v>47.465249999999997</v>
       </c>
-      <c r="M34" s="117"/>
+      <c r="M34" s="134"/>
       <c r="N34" s="13">
         <v>280</v>
       </c>
@@ -4420,7 +4586,7 @@
         <f t="shared" si="14"/>
         <v>39.519625000000019</v>
       </c>
-      <c r="M35" s="117"/>
+      <c r="M35" s="134"/>
       <c r="N35" s="13">
         <v>480</v>
       </c>
@@ -4474,7 +4640,7 @@
         <f t="shared" si="14"/>
         <v>55.930499999999995</v>
       </c>
-      <c r="M36" s="117"/>
+      <c r="M36" s="134"/>
       <c r="N36" s="13">
         <v>590</v>
       </c>
@@ -4551,7 +4717,7 @@
         <f t="shared" ref="L38:L43" si="17">K38-I38</f>
         <v>24.796975000000018</v>
       </c>
-      <c r="M38" s="117" t="s">
+      <c r="M38" s="134" t="s">
         <v>45</v>
       </c>
       <c r="N38" s="21">
@@ -4607,7 +4773,7 @@
         <f t="shared" si="17"/>
         <v>24.950450000000004</v>
       </c>
-      <c r="M39" s="117"/>
+      <c r="M39" s="134"/>
       <c r="N39" s="13">
         <v>160</v>
       </c>
@@ -4661,7 +4827,7 @@
         <f t="shared" si="17"/>
         <v>21.591537500000001</v>
       </c>
-      <c r="M40" s="117"/>
+      <c r="M40" s="134"/>
       <c r="N40" s="13"/>
       <c r="O40" s="11" t="s">
         <v>136</v>
@@ -4713,7 +4879,7 @@
         <f t="shared" si="17"/>
         <v>34.336550000000017</v>
       </c>
-      <c r="M41" s="117"/>
+      <c r="M41" s="134"/>
       <c r="N41" s="13">
         <v>340</v>
       </c>
@@ -4767,7 +4933,7 @@
         <f t="shared" si="17"/>
         <v>21.591537500000001</v>
       </c>
-      <c r="M42" s="117"/>
+      <c r="M42" s="134"/>
       <c r="N42" s="13"/>
       <c r="O42" s="11" t="s">
         <v>137</v>
@@ -4819,7 +4985,7 @@
         <f t="shared" si="17"/>
         <v>34.336550000000017</v>
       </c>
-      <c r="M43" s="117"/>
+      <c r="M43" s="134"/>
       <c r="N43" s="13">
         <v>340</v>
       </c>
@@ -4896,7 +5062,7 @@
         <f t="shared" ref="L45:L50" si="21">K45-I45</f>
         <v>61.054374999999993</v>
       </c>
-      <c r="M45" s="118" t="s">
+      <c r="M45" s="135" t="s">
         <v>141</v>
       </c>
       <c r="N45" s="13">
@@ -4950,7 +5116,7 @@
         <f t="shared" si="21"/>
         <v>37.158299999999997</v>
       </c>
-      <c r="M46" s="119"/>
+      <c r="M46" s="136"/>
       <c r="N46" s="13"/>
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
@@ -5000,7 +5166,7 @@
         <f t="shared" si="21"/>
         <v>40.13352500000002</v>
       </c>
-      <c r="M47" s="119"/>
+      <c r="M47" s="136"/>
       <c r="N47" s="13">
         <v>320</v>
       </c>
@@ -5054,7 +5220,7 @@
         <f t="shared" si="21"/>
         <v>42.341375000000028</v>
       </c>
-      <c r="M48" s="119"/>
+      <c r="M48" s="136"/>
       <c r="N48" s="13">
         <v>560</v>
       </c>
@@ -5108,7 +5274,7 @@
         <f t="shared" si="21"/>
         <v>74.70270000000005</v>
       </c>
-      <c r="M49" s="119"/>
+      <c r="M49" s="136"/>
       <c r="N49" s="13">
         <v>780</v>
       </c>
@@ -5160,7 +5326,7 @@
         <f t="shared" si="21"/>
         <v>70.346200000000067</v>
       </c>
-      <c r="M50" s="119"/>
+      <c r="M50" s="136"/>
       <c r="N50" s="13">
         <v>1080</v>
       </c>
@@ -5893,7 +6059,7 @@
         <f t="shared" si="26"/>
         <v>75.470075000000065</v>
       </c>
-      <c r="M65" s="115" t="s">
+      <c r="M65" s="132" t="s">
         <v>154</v>
       </c>
       <c r="N65" s="13">
@@ -5949,7 +6115,7 @@
         <f t="shared" si="26"/>
         <v>75.470075000000065</v>
       </c>
-      <c r="M66" s="116"/>
+      <c r="M66" s="133"/>
       <c r="N66" s="13">
         <v>490</v>
       </c>
@@ -6003,7 +6169,7 @@
         <f t="shared" si="26"/>
         <v>75.470075000000065</v>
       </c>
-      <c r="M67" s="116"/>
+      <c r="M67" s="133"/>
       <c r="N67" s="13">
         <v>490</v>
       </c>
@@ -6057,7 +6223,7 @@
         <f t="shared" si="26"/>
         <v>75.470075000000065</v>
       </c>
-      <c r="M68" s="116"/>
+      <c r="M68" s="133"/>
       <c r="N68" s="27">
         <v>490</v>
       </c>
@@ -6134,14 +6300,14 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="F1" s="138" t="s">
         <v>250</v>
       </c>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121" t="s">
+      <c r="G1" s="138"/>
+      <c r="H1" s="138" t="s">
         <v>252</v>
       </c>
-      <c r="I1" s="121"/>
+      <c r="I1" s="138"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -7231,14 +7397,14 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="121"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="138"/>
+      <c r="H1" s="131" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="121"/>
+      <c r="I1" s="138"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -7331,7 +7497,7 @@
         <f t="shared" ref="N3:N16" si="4">L3-I3</f>
         <v>67.158299999999997</v>
       </c>
-      <c r="O3" s="122" t="s">
+      <c r="O3" s="139" t="s">
         <v>162</v>
       </c>
       <c r="P3" s="40"/>
@@ -7386,7 +7552,7 @@
         <f t="shared" si="4"/>
         <v>67.158299999999997</v>
       </c>
-      <c r="O4" s="122"/>
+      <c r="O4" s="139"/>
       <c r="P4" s="42"/>
       <c r="Q4" s="42" t="s">
         <v>175</v>
@@ -7439,7 +7605,7 @@
         <f t="shared" si="4"/>
         <v>37.465249999999997</v>
       </c>
-      <c r="O5" s="122"/>
+      <c r="O5" s="139"/>
       <c r="P5" s="42"/>
       <c r="Q5" s="42" t="s">
         <v>176</v>
@@ -7492,7 +7658,7 @@
         <f t="shared" si="4"/>
         <v>63.108749999999986</v>
       </c>
-      <c r="O6" s="122"/>
+      <c r="O6" s="139"/>
       <c r="P6" s="42"/>
       <c r="Q6" s="42" t="s">
         <v>177</v>
@@ -7545,7 +7711,7 @@
         <f t="shared" si="4"/>
         <v>80.900900000000007</v>
       </c>
-      <c r="O7" s="122"/>
+      <c r="O7" s="139"/>
       <c r="P7" s="42"/>
       <c r="Q7" s="42" t="s">
         <v>178</v>
@@ -7598,7 +7764,7 @@
         <f t="shared" si="4"/>
         <v>67.158299999999997</v>
       </c>
-      <c r="O8" s="122"/>
+      <c r="O8" s="139"/>
       <c r="P8" s="42"/>
       <c r="Q8" s="42" t="s">
         <v>179</v>
@@ -7651,7 +7817,7 @@
         <f t="shared" si="4"/>
         <v>63.108749999999986</v>
       </c>
-      <c r="O9" s="122"/>
+      <c r="O9" s="139"/>
       <c r="P9" s="42"/>
       <c r="Q9" s="42" t="s">
         <v>180</v>
@@ -7704,7 +7870,7 @@
         <f t="shared" si="4"/>
         <v>47.465249999999997</v>
       </c>
-      <c r="O10" s="122"/>
+      <c r="O10" s="139"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="42" t="s">
         <v>175</v>
@@ -7757,7 +7923,7 @@
         <f t="shared" si="4"/>
         <v>63.108749999999986</v>
       </c>
-      <c r="O11" s="122"/>
+      <c r="O11" s="139"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="42">
         <v>400</v>
@@ -7810,7 +7976,7 @@
         <f t="shared" si="4"/>
         <v>61.514800000000008</v>
       </c>
-      <c r="O12" s="122"/>
+      <c r="O12" s="139"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="42" t="s">
         <v>181</v>
@@ -7863,7 +8029,7 @@
         <f t="shared" si="4"/>
         <v>61.514800000000008</v>
       </c>
-      <c r="O13" s="122"/>
+      <c r="O13" s="139"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="42" t="s">
         <v>175</v>
@@ -7899,7 +8065,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O14" s="122"/>
+      <c r="O14" s="139"/>
       <c r="P14" s="45"/>
       <c r="Q14" s="45"/>
       <c r="R14" s="46"/>
@@ -7930,7 +8096,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O15" s="122"/>
+      <c r="O15" s="139"/>
       <c r="P15" s="45"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="46"/>
@@ -7961,7 +8127,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O16" s="122"/>
+      <c r="O16" s="139"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="46"/>
@@ -8021,14 +8187,14 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="121"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="138"/>
+      <c r="H1" s="131" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="121"/>
+      <c r="I1" s="138"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -9724,14 +9890,14 @@
       <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="131"/>
+      <c r="H1" s="131" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="114"/>
+      <c r="I1" s="131"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -9822,7 +9988,7 @@
         <f t="shared" ref="L3:L17" si="3">K3-I3</f>
         <v>18.079149999999998</v>
       </c>
-      <c r="M3" s="122" t="s">
+      <c r="M3" s="139" t="s">
         <v>162</v>
       </c>
       <c r="N3" s="98">
@@ -9875,7 +10041,7 @@
         <f t="shared" si="3"/>
         <v>20.643500000000017</v>
       </c>
-      <c r="M4" s="122"/>
+      <c r="M4" s="139"/>
       <c r="N4" s="42"/>
       <c r="O4" s="99">
         <f t="shared" ref="O4:O17" si="5">N4*6.125*1.2+8</f>
@@ -9922,7 +10088,7 @@
         <f t="shared" si="3"/>
         <v>11.257400000000004</v>
       </c>
-      <c r="M5" s="122"/>
+      <c r="M5" s="139"/>
       <c r="N5" s="42"/>
       <c r="O5" s="99">
         <f t="shared" si="5"/>
@@ -9969,7 +10135,7 @@
         <f t="shared" si="3"/>
         <v>20.796975000000018</v>
       </c>
-      <c r="M6" s="122"/>
+      <c r="M6" s="139"/>
       <c r="N6" s="42"/>
       <c r="O6" s="99">
         <f t="shared" si="5"/>
@@ -10016,7 +10182,7 @@
         <f t="shared" si="3"/>
         <v>11.668275000000008</v>
       </c>
-      <c r="M7" s="122"/>
+      <c r="M7" s="139"/>
       <c r="N7" s="100">
         <v>11</v>
       </c>
@@ -10067,7 +10233,7 @@
         <f t="shared" si="3"/>
         <v>15.257400000000004</v>
       </c>
-      <c r="M8" s="122"/>
+      <c r="M8" s="139"/>
       <c r="N8" s="42"/>
       <c r="O8" s="99">
         <f t="shared" si="5"/>
@@ -10114,7 +10280,7 @@
         <f t="shared" si="3"/>
         <v>18.232624999999999</v>
       </c>
-      <c r="M9" s="122"/>
+      <c r="M9" s="139"/>
       <c r="N9" s="100">
         <v>11</v>
       </c>
@@ -10165,7 +10331,7 @@
         <f t="shared" si="3"/>
         <v>18.232624999999999</v>
       </c>
-      <c r="M10" s="122"/>
+      <c r="M10" s="139"/>
       <c r="N10" s="100">
         <v>11</v>
       </c>
@@ -10216,7 +10382,7 @@
         <f t="shared" si="3"/>
         <v>27.618725000000012</v>
       </c>
-      <c r="M11" s="122"/>
+      <c r="M11" s="139"/>
       <c r="N11" s="42"/>
       <c r="O11" s="99">
         <f t="shared" si="5"/>
@@ -10263,7 +10429,7 @@
         <f t="shared" si="3"/>
         <v>27.618725000000012</v>
       </c>
-      <c r="M12" s="122"/>
+      <c r="M12" s="139"/>
       <c r="N12" s="42"/>
       <c r="O12" s="99">
         <f t="shared" si="5"/>
@@ -10310,7 +10476,7 @@
         <f t="shared" si="3"/>
         <v>18.616312499999999</v>
       </c>
-      <c r="M13" s="122"/>
+      <c r="M13" s="139"/>
       <c r="N13" s="42"/>
       <c r="O13" s="99">
         <f t="shared" si="5"/>
@@ -10357,7 +10523,7 @@
         <f t="shared" si="3"/>
         <v>21.207850000000008</v>
       </c>
-      <c r="M14" s="122"/>
+      <c r="M14" s="139"/>
       <c r="N14" s="42"/>
       <c r="O14" s="99">
         <f t="shared" si="5"/>
@@ -10404,7 +10570,7 @@
         <f t="shared" si="3"/>
         <v>18.232624999999999</v>
       </c>
-      <c r="M15" s="122"/>
+      <c r="M15" s="139"/>
       <c r="N15" s="45"/>
       <c r="O15" s="99">
         <f t="shared" si="5"/>
@@ -10451,7 +10617,7 @@
         <f t="shared" si="3"/>
         <v>18.232624999999999</v>
       </c>
-      <c r="M16" s="122"/>
+      <c r="M16" s="139"/>
       <c r="N16" s="45"/>
       <c r="O16" s="99">
         <f t="shared" si="5"/>
@@ -10498,7 +10664,7 @@
         <f t="shared" si="3"/>
         <v>17.514800000000008</v>
       </c>
-      <c r="M17" s="122"/>
+      <c r="M17" s="139"/>
       <c r="N17" s="45"/>
       <c r="O17" s="99">
         <f t="shared" si="5"/>
@@ -10699,15 +10865,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P48"/>
+  <dimension ref="B1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" customWidth="1"/>
@@ -10730,14 +10898,14 @@
       <c r="E1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="131"/>
+      <c r="H1" s="131" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="114"/>
+      <c r="I1" s="131"/>
       <c r="J1" s="80" t="s">
         <v>258</v>
       </c>
@@ -10794,7 +10962,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="40">
-        <v>5101</v>
+        <v>6101</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>318</v>
@@ -10828,7 +10996,7 @@
         <f t="shared" ref="L3:L18" si="3">K3-I3</f>
         <v>218.00900000000024</v>
       </c>
-      <c r="M3" s="122" t="s">
+      <c r="M3" s="139" t="s">
         <v>162</v>
       </c>
       <c r="N3" s="98"/>
@@ -10843,7 +11011,7 @@
         <v>295</v>
       </c>
       <c r="C4" s="42">
-        <v>5102</v>
+        <v>6102</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>319</v>
@@ -10877,7 +11045,7 @@
         <f t="shared" si="3"/>
         <v>255.43499999999995</v>
       </c>
-      <c r="M4" s="122"/>
+      <c r="M4" s="139"/>
       <c r="N4" s="42"/>
       <c r="O4" s="99">
         <f t="shared" ref="O4:O17" si="5">N4*6.125*1.2+8</f>
@@ -10890,7 +11058,7 @@
         <v>295</v>
       </c>
       <c r="C5" s="40">
-        <v>5103</v>
+        <v>6103</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>320</v>
@@ -10924,7 +11092,7 @@
         <f t="shared" si="3"/>
         <v>186.72199999999998</v>
       </c>
-      <c r="M5" s="122"/>
+      <c r="M5" s="139"/>
       <c r="N5" s="42"/>
       <c r="O5" s="99">
         <f t="shared" si="5"/>
@@ -10937,7 +11105,7 @@
         <v>295</v>
       </c>
       <c r="C6" s="42">
-        <v>5104</v>
+        <v>6104</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>321</v>
@@ -10971,7 +11139,7 @@
         <f t="shared" si="3"/>
         <v>223.38062500000001</v>
       </c>
-      <c r="M6" s="122"/>
+      <c r="M6" s="139"/>
       <c r="N6" s="42"/>
       <c r="O6" s="99">
         <f t="shared" si="5"/>
@@ -10984,7 +11152,7 @@
         <v>295</v>
       </c>
       <c r="C7" s="40">
-        <v>5105</v>
+        <v>6105</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>322</v>
@@ -11018,7 +11186,7 @@
         <f t="shared" si="3"/>
         <v>223.38062500000001</v>
       </c>
-      <c r="M7" s="122"/>
+      <c r="M7" s="139"/>
       <c r="N7" s="100"/>
       <c r="O7" s="99">
         <f t="shared" si="5"/>
@@ -11031,7 +11199,7 @@
         <v>295</v>
       </c>
       <c r="C8" s="42">
-        <v>5106</v>
+        <v>6106</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>315</v>
@@ -11065,7 +11233,7 @@
         <f t="shared" si="3"/>
         <v>127.21749999999997</v>
       </c>
-      <c r="M8" s="122"/>
+      <c r="M8" s="139"/>
       <c r="N8" s="42"/>
       <c r="O8" s="99">
         <f t="shared" si="5"/>
@@ -11078,7 +11246,7 @@
         <v>295</v>
       </c>
       <c r="C9" s="40">
-        <v>5107</v>
+        <v>6107</v>
       </c>
       <c r="D9" s="42" t="s">
         <v>323</v>
@@ -11112,7 +11280,7 @@
         <f t="shared" si="3"/>
         <v>127.21749999999997</v>
       </c>
-      <c r="M9" s="122"/>
+      <c r="M9" s="139"/>
       <c r="N9" s="100"/>
       <c r="O9" s="99">
         <f t="shared" si="5"/>
@@ -11125,7 +11293,7 @@
         <v>295</v>
       </c>
       <c r="C10" s="42">
-        <v>5108</v>
+        <v>6108</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>316</v>
@@ -11159,7 +11327,7 @@
         <f t="shared" si="3"/>
         <v>104.39575000000002</v>
       </c>
-      <c r="M10" s="122"/>
+      <c r="M10" s="139"/>
       <c r="N10" s="100">
         <v>60</v>
       </c>
@@ -11176,7 +11344,7 @@
         <v>295</v>
       </c>
       <c r="C11" s="40">
-        <v>5109</v>
+        <v>6109</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>317</v>
@@ -11210,7 +11378,7 @@
         <f t="shared" si="3"/>
         <v>104.39575000000002</v>
       </c>
-      <c r="M11" s="122"/>
+      <c r="M11" s="139"/>
       <c r="N11" s="42">
         <v>60</v>
       </c>
@@ -11227,7 +11395,7 @@
         <v>295</v>
       </c>
       <c r="C12" s="42">
-        <v>5110</v>
+        <v>6110</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>324</v>
@@ -11261,7 +11429,7 @@
         <f t="shared" si="3"/>
         <v>225.68275000000006</v>
       </c>
-      <c r="M12" s="122"/>
+      <c r="M12" s="139"/>
       <c r="N12" s="42">
         <v>80</v>
       </c>
@@ -11278,7 +11446,7 @@
         <v>295</v>
       </c>
       <c r="C13" s="40">
-        <v>5111</v>
+        <v>6111</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>325</v>
@@ -11312,7 +11480,7 @@
         <f t="shared" si="3"/>
         <v>225.68275000000006</v>
       </c>
-      <c r="M13" s="122"/>
+      <c r="M13" s="139"/>
       <c r="N13" s="42">
         <v>80</v>
       </c>
@@ -11329,7 +11497,7 @@
         <v>295</v>
       </c>
       <c r="C14" s="42">
-        <v>5112</v>
+        <v>6112</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>326</v>
@@ -11363,7 +11531,7 @@
         <f t="shared" si="3"/>
         <v>127.21749999999997</v>
       </c>
-      <c r="M14" s="122"/>
+      <c r="M14" s="139"/>
       <c r="N14" s="42"/>
       <c r="O14" s="99">
         <f t="shared" si="5"/>
@@ -11376,7 +11544,7 @@
         <v>295</v>
       </c>
       <c r="C15" s="40">
-        <v>5113</v>
+        <v>6113</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>327</v>
@@ -11410,7 +11578,7 @@
         <f t="shared" si="3"/>
         <v>94.395750000000021</v>
       </c>
-      <c r="M15" s="122"/>
+      <c r="M15" s="139"/>
       <c r="N15" s="45">
         <v>60</v>
       </c>
@@ -11427,7 +11595,7 @@
         <v>295</v>
       </c>
       <c r="C16" s="42">
-        <v>5114</v>
+        <v>6114</v>
       </c>
       <c r="D16" s="42" t="s">
         <v>328</v>
@@ -11461,7 +11629,7 @@
         <f t="shared" si="3"/>
         <v>94.395750000000021</v>
       </c>
-      <c r="M16" s="122"/>
+      <c r="M16" s="139"/>
       <c r="N16" s="45">
         <v>60</v>
       </c>
@@ -11474,11 +11642,11 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="22" customHeight="1">
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="122" t="s">
         <v>295</v>
       </c>
-      <c r="C17" s="130">
-        <v>5115</v>
+      <c r="C17" s="40">
+        <v>6115</v>
       </c>
       <c r="D17" s="45" t="s">
         <v>329</v>
@@ -11501,7 +11669,7 @@
         <f t="shared" si="2"/>
         <v>604.60424999999998</v>
       </c>
-      <c r="J17" s="131">
+      <c r="J17" s="124">
         <f t="shared" si="4"/>
         <v>703.29488749999996</v>
       </c>
@@ -11512,11 +11680,11 @@
         <f t="shared" si="3"/>
         <v>94.395750000000021</v>
       </c>
-      <c r="M17" s="122"/>
+      <c r="M17" s="139"/>
       <c r="N17" s="45">
         <v>60</v>
       </c>
-      <c r="O17" s="132">
+      <c r="O17" s="125">
         <f t="shared" si="5"/>
         <v>449</v>
       </c>
@@ -11524,12 +11692,12 @@
         <v>499</v>
       </c>
     </row>
-    <row r="18" spans="2:16" s="133" customFormat="1" ht="22" customHeight="1">
-      <c r="B18" s="129" t="s">
+    <row r="18" spans="2:16" s="126" customFormat="1" ht="22" customHeight="1">
+      <c r="B18" s="122" t="s">
         <v>295</v>
       </c>
       <c r="C18" s="42">
-        <v>5116</v>
+        <v>6116</v>
       </c>
       <c r="D18" s="42" t="s">
         <v>330</v>
@@ -11544,7 +11712,7 @@
         <f t="shared" si="0"/>
         <v>736.19999999999993</v>
       </c>
-      <c r="H18" s="134">
+      <c r="H18" s="127">
         <f t="shared" si="1"/>
         <v>131.4</v>
       </c>
@@ -11552,38 +11720,38 @@
         <f t="shared" si="2"/>
         <v>806.13900000000001</v>
       </c>
-      <c r="J18" s="123">
+      <c r="J18" s="116">
         <f t="shared" si="4"/>
         <v>935.05984999999998</v>
       </c>
       <c r="K18" s="102">
         <v>959</v>
       </c>
-      <c r="L18" s="135">
+      <c r="L18" s="128">
         <f t="shared" si="3"/>
         <v>152.86099999999999</v>
       </c>
-      <c r="M18" s="136"/>
+      <c r="M18" s="129"/>
       <c r="N18" s="42"/>
-      <c r="O18" s="137"/>
+      <c r="O18" s="130"/>
       <c r="P18" s="113"/>
     </row>
-    <row r="19" spans="2:16" s="128" customFormat="1" ht="22" customHeight="1">
-      <c r="B19" s="129"/>
-      <c r="C19" s="130"/>
+    <row r="19" spans="2:16" s="121" customFormat="1" ht="22" customHeight="1">
+      <c r="B19" s="122"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
       <c r="F19" s="45"/>
       <c r="G19" s="62"/>
       <c r="H19" s="56"/>
       <c r="I19" s="62"/>
-      <c r="J19" s="123"/>
+      <c r="J19" s="116"/>
       <c r="K19" s="103"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="125"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="118"/>
       <c r="N19" s="45"/>
-      <c r="O19" s="126"/>
-      <c r="P19" s="127"/>
+      <c r="O19" s="119"/>
+      <c r="P19" s="120"/>
     </row>
     <row r="20" spans="2:16" ht="22" customHeight="1">
       <c r="J20" s="81"/>
@@ -11593,7 +11761,7 @@
         <v>301</v>
       </c>
       <c r="C21" s="40">
-        <v>5201</v>
+        <v>6201</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>314</v>
@@ -11639,7 +11807,7 @@
         <v>301</v>
       </c>
       <c r="C22" s="42">
-        <v>5202</v>
+        <v>6202</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>304</v>
@@ -11685,7 +11853,7 @@
         <v>301</v>
       </c>
       <c r="C23" s="40">
-        <v>5203</v>
+        <v>6203</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>303</v>
@@ -11731,7 +11899,7 @@
         <v>301</v>
       </c>
       <c r="C24" s="42">
-        <v>5204</v>
+        <v>6204</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>306</v>
@@ -11777,7 +11945,7 @@
         <v>301</v>
       </c>
       <c r="C25" s="40">
-        <v>5205</v>
+        <v>6205</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>305</v>
@@ -11823,7 +11991,7 @@
         <v>301</v>
       </c>
       <c r="C26" s="42">
-        <v>5206</v>
+        <v>6206</v>
       </c>
       <c r="D26" s="40" t="s">
         <v>305</v>
@@ -11869,7 +12037,7 @@
         <v>301</v>
       </c>
       <c r="C27" s="40">
-        <v>5207</v>
+        <v>6207</v>
       </c>
       <c r="D27" s="40" t="s">
         <v>308</v>
@@ -11915,7 +12083,7 @@
         <v>301</v>
       </c>
       <c r="C28" s="42">
-        <v>5208</v>
+        <v>6208</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>309</v>
@@ -11961,7 +12129,7 @@
         <v>301</v>
       </c>
       <c r="C29" s="40">
-        <v>5209</v>
+        <v>6209</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>312</v>
@@ -12007,7 +12175,7 @@
         <v>301</v>
       </c>
       <c r="C30" s="42">
-        <v>5210</v>
+        <v>6210</v>
       </c>
       <c r="D30" s="40" t="s">
         <v>313</v>
@@ -12050,146 +12218,628 @@
     </row>
     <row r="31" spans="2:16" ht="22" customHeight="1">
       <c r="J31" s="81">
-        <f t="shared" ref="J20:J48" si="18">I31*1.15</f>
+        <f t="shared" ref="J31:J61" si="18">I31*1.15</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="22" customHeight="1">
+      <c r="B32" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C32" s="40">
+        <v>6301</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="F32" s="40">
+        <v>43</v>
+      </c>
+      <c r="G32" s="66">
+        <f t="shared" ref="G32:G40" si="19">F32*6.135</f>
+        <v>263.80500000000001</v>
+      </c>
+      <c r="H32" s="60">
+        <f t="shared" ref="H32:H40" si="20">F32*(1+0.095)</f>
+        <v>47.085000000000001</v>
+      </c>
+      <c r="I32" s="66">
+        <f t="shared" ref="I32:I40" si="21">H32*6.135</f>
+        <v>288.86647499999998</v>
+      </c>
       <c r="J32" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="10:16" ht="22" customHeight="1">
+        <f>I32*1.15+8</f>
+        <v>340.19644624999995</v>
+      </c>
+      <c r="K32" s="101">
+        <v>341</v>
+      </c>
+      <c r="L32" s="110">
+        <f t="shared" ref="L32:L40" si="22">K32-I32</f>
+        <v>52.13352500000002</v>
+      </c>
+      <c r="N32" s="98"/>
+      <c r="O32" s="99">
+        <f>N32*6.125*1.2+8</f>
+        <v>8</v>
+      </c>
+      <c r="P32" s="105"/>
+    </row>
+    <row r="33" spans="2:16" ht="22" customHeight="1">
+      <c r="B33" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C33" s="42">
+        <v>6302</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" s="42">
+        <v>43</v>
+      </c>
+      <c r="G33" s="62">
+        <f t="shared" si="19"/>
+        <v>263.80500000000001</v>
+      </c>
+      <c r="H33" s="56">
+        <f t="shared" si="20"/>
+        <v>47.085000000000001</v>
+      </c>
+      <c r="I33" s="62">
+        <f t="shared" si="21"/>
+        <v>288.86647499999998</v>
+      </c>
       <c r="J33" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="10:16" ht="22" customHeight="1">
+        <f t="shared" ref="J33:J40" si="23">I33*1.15+8</f>
+        <v>340.19644624999995</v>
+      </c>
+      <c r="K33" s="102">
+        <v>341</v>
+      </c>
+      <c r="L33" s="110">
+        <f t="shared" si="22"/>
+        <v>52.13352500000002</v>
+      </c>
+      <c r="N33" s="42"/>
+      <c r="O33" s="99">
+        <f t="shared" ref="O33:O40" si="24">N33*6.125*1.2+8</f>
+        <v>8</v>
+      </c>
+      <c r="P33" s="106"/>
+    </row>
+    <row r="34" spans="2:16" ht="22" customHeight="1">
+      <c r="B34" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" s="40">
+        <v>6303</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F34" s="42">
+        <v>50</v>
+      </c>
+      <c r="G34" s="62">
+        <f t="shared" si="19"/>
+        <v>306.75</v>
+      </c>
+      <c r="H34" s="56">
+        <f t="shared" si="20"/>
+        <v>54.75</v>
+      </c>
+      <c r="I34" s="62">
+        <f t="shared" si="21"/>
+        <v>335.89125000000001</v>
+      </c>
       <c r="J34" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>394.27493749999996</v>
+      </c>
+      <c r="K34" s="102">
+        <v>399</v>
+      </c>
+      <c r="L34" s="110">
+        <f t="shared" si="22"/>
+        <v>63.108749999999986</v>
+      </c>
+      <c r="N34" s="42"/>
+      <c r="O34" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P34" s="106"/>
+    </row>
+    <row r="35" spans="2:16" ht="22" customHeight="1">
+      <c r="B35" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C35" s="42">
+        <v>6304</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F35" s="42">
+        <v>43</v>
+      </c>
+      <c r="G35" s="62">
+        <f t="shared" si="19"/>
+        <v>263.80500000000001</v>
+      </c>
+      <c r="H35" s="56">
+        <f t="shared" si="20"/>
+        <v>47.085000000000001</v>
+      </c>
+      <c r="I35" s="62">
+        <f t="shared" si="21"/>
+        <v>288.86647499999998</v>
+      </c>
       <c r="J35" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="P35"/>
-    </row>
-    <row r="36" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>340.19644624999995</v>
+      </c>
+      <c r="K35" s="102">
+        <v>341</v>
+      </c>
+      <c r="L35" s="110">
+        <f t="shared" si="22"/>
+        <v>52.13352500000002</v>
+      </c>
+      <c r="N35" s="42"/>
+      <c r="O35" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P35" s="106"/>
+    </row>
+    <row r="36" spans="2:16" ht="22" customHeight="1">
+      <c r="B36" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C36" s="40">
+        <v>6305</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F36" s="42">
+        <v>49</v>
+      </c>
+      <c r="G36" s="62">
+        <f t="shared" si="19"/>
+        <v>300.61500000000001</v>
+      </c>
+      <c r="H36" s="56">
+        <f t="shared" si="20"/>
+        <v>53.655000000000001</v>
+      </c>
+      <c r="I36" s="62">
+        <f t="shared" si="21"/>
+        <v>329.17342500000001</v>
+      </c>
       <c r="J36" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="P36"/>
-    </row>
-    <row r="37" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>386.54943874999998</v>
+      </c>
+      <c r="K36" s="102">
+        <v>389</v>
+      </c>
+      <c r="L36" s="110">
+        <f t="shared" si="22"/>
+        <v>59.826574999999991</v>
+      </c>
+      <c r="N36" s="100"/>
+      <c r="O36" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P36" s="106"/>
+    </row>
+    <row r="37" spans="2:16" ht="22" customHeight="1">
+      <c r="B37" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C37" s="42">
+        <v>6306</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>347</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F37" s="42">
+        <v>53</v>
+      </c>
+      <c r="G37" s="62">
+        <f t="shared" ref="G37" si="25">F37*6.135</f>
+        <v>325.15499999999997</v>
+      </c>
+      <c r="H37" s="56">
+        <f t="shared" ref="H37" si="26">F37*(1+0.095)</f>
+        <v>58.034999999999997</v>
+      </c>
+      <c r="I37" s="62">
+        <f t="shared" ref="I37" si="27">H37*6.135</f>
+        <v>356.04472499999997</v>
+      </c>
       <c r="J37" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="P37"/>
-    </row>
-    <row r="38" spans="10:16" ht="17">
+        <f t="shared" ref="J37" si="28">I37*1.15+8</f>
+        <v>417.45143374999992</v>
+      </c>
+      <c r="K37" s="102">
+        <v>419</v>
+      </c>
+      <c r="L37" s="110">
+        <f t="shared" ref="L37" si="29">K37-I37</f>
+        <v>62.955275000000029</v>
+      </c>
+      <c r="N37" s="42"/>
+      <c r="O37" s="99">
+        <f t="shared" ref="O37" si="30">N37*6.125*1.2+8</f>
+        <v>8</v>
+      </c>
+      <c r="P37" s="106"/>
+    </row>
+    <row r="38" spans="2:16" ht="22" customHeight="1">
+      <c r="B38" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C38" s="40">
+        <v>6307</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F38" s="42">
+        <v>53</v>
+      </c>
+      <c r="G38" s="62">
+        <f t="shared" si="19"/>
+        <v>325.15499999999997</v>
+      </c>
+      <c r="H38" s="56">
+        <f t="shared" si="20"/>
+        <v>58.034999999999997</v>
+      </c>
+      <c r="I38" s="62">
+        <f t="shared" si="21"/>
+        <v>356.04472499999997</v>
+      </c>
       <c r="J38" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="P38"/>
-    </row>
-    <row r="39" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>417.45143374999992</v>
+      </c>
+      <c r="K38" s="102">
+        <v>419</v>
+      </c>
+      <c r="L38" s="110">
+        <f t="shared" si="22"/>
+        <v>62.955275000000029</v>
+      </c>
+      <c r="N38" s="42"/>
+      <c r="O38" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P38" s="106"/>
+    </row>
+    <row r="39" spans="2:16" ht="22" customHeight="1">
+      <c r="B39" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C39" s="42">
+        <v>6308</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>341</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F39" s="42">
+        <v>44</v>
+      </c>
+      <c r="G39" s="62">
+        <f t="shared" si="19"/>
+        <v>269.94</v>
+      </c>
+      <c r="H39" s="56">
+        <f t="shared" si="20"/>
+        <v>48.18</v>
+      </c>
+      <c r="I39" s="62">
+        <f t="shared" si="21"/>
+        <v>295.58429999999998</v>
+      </c>
       <c r="J39" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="P39"/>
-    </row>
-    <row r="40" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>347.92194499999994</v>
+      </c>
+      <c r="K39" s="102">
+        <v>349</v>
+      </c>
+      <c r="L39" s="110">
+        <f t="shared" si="22"/>
+        <v>53.415700000000015</v>
+      </c>
+      <c r="N39" s="100"/>
+      <c r="O39" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P39" s="106"/>
+    </row>
+    <row r="40" spans="2:16" ht="22" customHeight="1">
+      <c r="B40" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C40" s="40">
+        <v>6309</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>342</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F40" s="42">
+        <v>48</v>
+      </c>
+      <c r="G40" s="62">
+        <f t="shared" si="19"/>
+        <v>294.48</v>
+      </c>
+      <c r="H40" s="56">
+        <f t="shared" si="20"/>
+        <v>52.56</v>
+      </c>
+      <c r="I40" s="62">
+        <f t="shared" si="21"/>
+        <v>322.4556</v>
+      </c>
       <c r="J40" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="P40"/>
-    </row>
-    <row r="41" spans="10:16" ht="17">
+        <f t="shared" si="23"/>
+        <v>378.82393999999999</v>
+      </c>
+      <c r="K40" s="102">
+        <v>379</v>
+      </c>
+      <c r="L40" s="110">
+        <f t="shared" si="22"/>
+        <v>56.544399999999996</v>
+      </c>
+      <c r="N40" s="100"/>
+      <c r="O40" s="99">
+        <f t="shared" si="24"/>
+        <v>8</v>
+      </c>
+      <c r="P40" s="106"/>
+    </row>
+    <row r="41" spans="2:16" ht="22" customHeight="1">
+      <c r="B41" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C41" s="42">
+        <v>6310</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>343</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="F41" s="40">
+        <v>43</v>
+      </c>
+      <c r="G41" s="66">
+        <f t="shared" ref="G41:G44" si="31">F41*6.135</f>
+        <v>263.80500000000001</v>
+      </c>
+      <c r="H41" s="60">
+        <f t="shared" ref="H41:H44" si="32">F41*(1+0.095)</f>
+        <v>47.085000000000001</v>
+      </c>
+      <c r="I41" s="66">
+        <f t="shared" ref="I41:I44" si="33">H41*6.135</f>
+        <v>288.86647499999998</v>
+      </c>
       <c r="J41" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="P41"/>
-    </row>
-    <row r="42" spans="10:16" ht="17">
+        <f>I41*1.15+8</f>
+        <v>340.19644624999995</v>
+      </c>
+      <c r="K41" s="101">
+        <v>341</v>
+      </c>
+      <c r="L41" s="110">
+        <f t="shared" ref="L41:L44" si="34">K41-I41</f>
+        <v>52.13352500000002</v>
+      </c>
+      <c r="N41" s="98"/>
+      <c r="O41" s="99">
+        <f>N41*6.125*1.2+8</f>
+        <v>8</v>
+      </c>
+      <c r="P41" s="105"/>
+    </row>
+    <row r="42" spans="2:16" ht="22" customHeight="1">
+      <c r="B42" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C42" s="40">
+        <v>6311</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="E42" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="F42" s="42">
+        <v>46</v>
+      </c>
+      <c r="G42" s="62">
+        <f t="shared" si="31"/>
+        <v>282.20999999999998</v>
+      </c>
+      <c r="H42" s="56">
+        <f t="shared" si="32"/>
+        <v>50.37</v>
+      </c>
+      <c r="I42" s="62">
+        <f t="shared" si="33"/>
+        <v>309.01994999999999</v>
+      </c>
       <c r="J42" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="P42"/>
-    </row>
-    <row r="43" spans="10:16" ht="17">
+        <f t="shared" ref="J42:J44" si="35">I42*1.15+8</f>
+        <v>363.37294249999997</v>
+      </c>
+      <c r="K42" s="102">
+        <v>369</v>
+      </c>
+      <c r="L42" s="110">
+        <f t="shared" si="34"/>
+        <v>59.980050000000006</v>
+      </c>
+      <c r="N42" s="42"/>
+      <c r="O42" s="99">
+        <f t="shared" ref="O42:O44" si="36">N42*6.125*1.2+8</f>
+        <v>8</v>
+      </c>
+      <c r="P42" s="106"/>
+    </row>
+    <row r="43" spans="2:16" ht="22" customHeight="1">
+      <c r="B43" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C43" s="42">
+        <v>6312</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>345</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F43" s="42">
+        <v>49</v>
+      </c>
+      <c r="G43" s="62">
+        <f t="shared" si="31"/>
+        <v>300.61500000000001</v>
+      </c>
+      <c r="H43" s="56">
+        <f t="shared" si="32"/>
+        <v>53.655000000000001</v>
+      </c>
+      <c r="I43" s="62">
+        <f t="shared" si="33"/>
+        <v>329.17342500000001</v>
+      </c>
       <c r="J43" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="P43"/>
-    </row>
-    <row r="44" spans="10:16" ht="17">
+        <f t="shared" si="35"/>
+        <v>386.54943874999998</v>
+      </c>
+      <c r="K43" s="102">
+        <v>389</v>
+      </c>
+      <c r="L43" s="110">
+        <f t="shared" si="34"/>
+        <v>59.826574999999991</v>
+      </c>
+      <c r="N43" s="42"/>
+      <c r="O43" s="99">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="P43" s="106"/>
+    </row>
+    <row r="44" spans="2:16" ht="22" customHeight="1">
+      <c r="B44" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C44" s="40">
+        <v>6313</v>
+      </c>
+      <c r="D44" s="40" t="s">
+        <v>346</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="F44" s="42">
+        <v>58</v>
+      </c>
+      <c r="G44" s="62">
+        <f t="shared" si="31"/>
+        <v>355.83</v>
+      </c>
+      <c r="H44" s="56">
+        <f t="shared" si="32"/>
+        <v>63.51</v>
+      </c>
+      <c r="I44" s="62">
+        <f t="shared" si="33"/>
+        <v>389.63385</v>
+      </c>
       <c r="J44" s="81">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="P44"/>
-    </row>
-    <row r="45" spans="10:16" ht="17">
+        <f t="shared" si="35"/>
+        <v>456.07892749999996</v>
+      </c>
+      <c r="K44" s="102">
+        <v>459</v>
+      </c>
+      <c r="L44" s="110">
+        <f t="shared" si="34"/>
+        <v>69.366150000000005</v>
+      </c>
+      <c r="N44" s="42"/>
+      <c r="O44" s="99">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="P44" s="106"/>
+    </row>
+    <row r="45" spans="2:16" ht="22" customHeight="1">
+      <c r="B45" s="140"/>
       <c r="J45" s="81">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="P45"/>
-    </row>
-    <row r="46" spans="10:16" ht="17">
+    </row>
+    <row r="46" spans="2:16" ht="22" customHeight="1">
       <c r="J46" s="81">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="P46"/>
-    </row>
-    <row r="47" spans="10:16" ht="17">
+    </row>
+    <row r="47" spans="2:16" ht="22" customHeight="1">
       <c r="J47" s="81">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="P47"/>
-    </row>
-    <row r="48" spans="10:16" ht="17">
+    </row>
+    <row r="48" spans="2:16" ht="17">
       <c r="J48" s="81">
         <f t="shared" si="18"/>
         <v>0</v>
@@ -12197,6 +12847,123 @@
       <c r="K48"/>
       <c r="L48"/>
       <c r="P48"/>
+    </row>
+    <row r="49" spans="10:16" ht="17">
+      <c r="J49" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="10:16" ht="17">
+      <c r="J50" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="10:16" ht="17">
+      <c r="J51" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="P51"/>
+    </row>
+    <row r="52" spans="10:16" ht="17">
+      <c r="J52" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="P52"/>
+    </row>
+    <row r="53" spans="10:16" ht="17">
+      <c r="J53" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="P53"/>
+    </row>
+    <row r="54" spans="10:16" ht="17">
+      <c r="J54" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="P54"/>
+    </row>
+    <row r="55" spans="10:16" ht="17">
+      <c r="J55" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="P55"/>
+    </row>
+    <row r="56" spans="10:16" ht="17">
+      <c r="J56" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="P56"/>
+    </row>
+    <row r="57" spans="10:16" ht="17">
+      <c r="J57" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="P57"/>
+    </row>
+    <row r="58" spans="10:16" ht="17">
+      <c r="J58" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="P58"/>
+    </row>
+    <row r="59" spans="10:16" ht="17">
+      <c r="J59" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="P59"/>
+    </row>
+    <row r="60" spans="10:16" ht="17">
+      <c r="J60" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="P60"/>
+    </row>
+    <row r="61" spans="10:16" ht="17">
+      <c r="J61" s="81">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="P61"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -12213,4 +12980,551 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="65" customHeight="1">
+      <c r="B1" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="115" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="115" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="115" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="131" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131" t="s">
+        <v>253</v>
+      </c>
+      <c r="I1" s="131"/>
+      <c r="J1" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="K1" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="109" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="115" t="s">
+        <v>268</v>
+      </c>
+      <c r="N1" s="115" t="s">
+        <v>273</v>
+      </c>
+      <c r="O1" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="P1" s="104" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" ht="65" customHeight="1">
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="114" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="H2" s="114" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="80" t="s">
+        <v>257</v>
+      </c>
+      <c r="K2" s="93"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115" t="s">
+        <v>275</v>
+      </c>
+      <c r="P2" s="104"/>
+    </row>
+    <row r="3" spans="2:16" ht="22" customHeight="1">
+      <c r="B3" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="40">
+        <v>7101</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" s="40">
+        <v>79</v>
+      </c>
+      <c r="G3" s="66">
+        <f t="shared" ref="G3:G11" si="0">F3*6.135</f>
+        <v>484.66499999999996</v>
+      </c>
+      <c r="H3" s="60">
+        <f t="shared" ref="H3:H11" si="1">F3*(1+0.095)</f>
+        <v>86.504999999999995</v>
+      </c>
+      <c r="I3" s="66">
+        <f t="shared" ref="I3:I11" si="2">H3*6.135</f>
+        <v>530.70817499999998</v>
+      </c>
+      <c r="J3" s="81">
+        <f>I3*1.15+8</f>
+        <v>618.31440124999995</v>
+      </c>
+      <c r="K3" s="101">
+        <v>619</v>
+      </c>
+      <c r="L3" s="110">
+        <f t="shared" ref="L3:L11" si="3">K3-I3</f>
+        <v>88.291825000000017</v>
+      </c>
+      <c r="N3" s="98">
+        <v>59</v>
+      </c>
+      <c r="O3" s="99">
+        <f>N3*6.125*1.2+8</f>
+        <v>441.65</v>
+      </c>
+      <c r="P3" s="105">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="22" customHeight="1">
+      <c r="B4" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C4" s="42">
+        <v>7102</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F4" s="42">
+        <v>79</v>
+      </c>
+      <c r="G4" s="62">
+        <f t="shared" si="0"/>
+        <v>484.66499999999996</v>
+      </c>
+      <c r="H4" s="56">
+        <f t="shared" si="1"/>
+        <v>86.504999999999995</v>
+      </c>
+      <c r="I4" s="62">
+        <f t="shared" si="2"/>
+        <v>530.70817499999998</v>
+      </c>
+      <c r="J4" s="81">
+        <f t="shared" ref="J4:J11" si="4">I4*1.15+8</f>
+        <v>618.31440124999995</v>
+      </c>
+      <c r="K4" s="102">
+        <v>619</v>
+      </c>
+      <c r="L4" s="110">
+        <f t="shared" si="3"/>
+        <v>88.291825000000017</v>
+      </c>
+      <c r="N4" s="42">
+        <v>59</v>
+      </c>
+      <c r="O4" s="99">
+        <f t="shared" ref="O4:O11" si="5">N4*6.125*1.2+8</f>
+        <v>441.65</v>
+      </c>
+      <c r="P4" s="106">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="22" customHeight="1">
+      <c r="B5" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="40">
+        <v>7103</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>351</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F5" s="42">
+        <v>79</v>
+      </c>
+      <c r="G5" s="62">
+        <f t="shared" si="0"/>
+        <v>484.66499999999996</v>
+      </c>
+      <c r="H5" s="56">
+        <f t="shared" si="1"/>
+        <v>86.504999999999995</v>
+      </c>
+      <c r="I5" s="62">
+        <f t="shared" si="2"/>
+        <v>530.70817499999998</v>
+      </c>
+      <c r="J5" s="81">
+        <f t="shared" si="4"/>
+        <v>618.31440124999995</v>
+      </c>
+      <c r="K5" s="102">
+        <v>619</v>
+      </c>
+      <c r="L5" s="110">
+        <f t="shared" si="3"/>
+        <v>88.291825000000017</v>
+      </c>
+      <c r="N5" s="42">
+        <v>59</v>
+      </c>
+      <c r="O5" s="99">
+        <f t="shared" si="5"/>
+        <v>441.65</v>
+      </c>
+      <c r="P5" s="106">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="22" customHeight="1">
+      <c r="B6" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C6" s="42">
+        <v>7104</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F6" s="42">
+        <v>79</v>
+      </c>
+      <c r="G6" s="62">
+        <f t="shared" si="0"/>
+        <v>484.66499999999996</v>
+      </c>
+      <c r="H6" s="56">
+        <f t="shared" si="1"/>
+        <v>86.504999999999995</v>
+      </c>
+      <c r="I6" s="62">
+        <f t="shared" si="2"/>
+        <v>530.70817499999998</v>
+      </c>
+      <c r="J6" s="81">
+        <f t="shared" si="4"/>
+        <v>618.31440124999995</v>
+      </c>
+      <c r="K6" s="102">
+        <v>619</v>
+      </c>
+      <c r="L6" s="110">
+        <f t="shared" si="3"/>
+        <v>88.291825000000017</v>
+      </c>
+      <c r="N6" s="42">
+        <v>59</v>
+      </c>
+      <c r="O6" s="99">
+        <f t="shared" si="5"/>
+        <v>441.65</v>
+      </c>
+      <c r="P6" s="106">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="22" customHeight="1">
+      <c r="B7" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" s="40">
+        <v>7105</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F7" s="42">
+        <v>129</v>
+      </c>
+      <c r="G7" s="62">
+        <f t="shared" si="0"/>
+        <v>791.41499999999996</v>
+      </c>
+      <c r="H7" s="56">
+        <f t="shared" si="1"/>
+        <v>141.255</v>
+      </c>
+      <c r="I7" s="62">
+        <f t="shared" si="2"/>
+        <v>866.599425</v>
+      </c>
+      <c r="J7" s="81">
+        <f t="shared" si="4"/>
+        <v>1004.5893387499999</v>
+      </c>
+      <c r="K7" s="102">
+        <v>1009</v>
+      </c>
+      <c r="L7" s="110">
+        <f t="shared" si="3"/>
+        <v>142.400575</v>
+      </c>
+      <c r="N7" s="100"/>
+      <c r="O7" s="99">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P7" s="106"/>
+    </row>
+    <row r="8" spans="2:16" ht="22" customHeight="1">
+      <c r="B8" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C8" s="42">
+        <v>7106</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F8" s="42">
+        <v>129</v>
+      </c>
+      <c r="G8" s="62">
+        <f t="shared" si="0"/>
+        <v>791.41499999999996</v>
+      </c>
+      <c r="H8" s="56">
+        <f t="shared" si="1"/>
+        <v>141.255</v>
+      </c>
+      <c r="I8" s="62">
+        <f t="shared" si="2"/>
+        <v>866.599425</v>
+      </c>
+      <c r="J8" s="81">
+        <f t="shared" si="4"/>
+        <v>1004.5893387499999</v>
+      </c>
+      <c r="K8" s="102">
+        <v>1009</v>
+      </c>
+      <c r="L8" s="110">
+        <f t="shared" si="3"/>
+        <v>142.400575</v>
+      </c>
+      <c r="N8" s="42"/>
+      <c r="O8" s="99">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P8" s="106"/>
+    </row>
+    <row r="9" spans="2:16" ht="22" customHeight="1">
+      <c r="B9" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" s="40">
+        <v>7107</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="F9" s="42">
+        <v>129</v>
+      </c>
+      <c r="G9" s="62">
+        <f t="shared" si="0"/>
+        <v>791.41499999999996</v>
+      </c>
+      <c r="H9" s="56">
+        <f t="shared" si="1"/>
+        <v>141.255</v>
+      </c>
+      <c r="I9" s="62">
+        <f t="shared" si="2"/>
+        <v>866.599425</v>
+      </c>
+      <c r="J9" s="81">
+        <f t="shared" si="4"/>
+        <v>1004.5893387499999</v>
+      </c>
+      <c r="K9" s="102">
+        <v>1009</v>
+      </c>
+      <c r="L9" s="110">
+        <f t="shared" si="3"/>
+        <v>142.400575</v>
+      </c>
+      <c r="N9" s="100"/>
+      <c r="O9" s="99">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P9" s="106"/>
+    </row>
+    <row r="10" spans="2:16" ht="22" customHeight="1">
+      <c r="B10" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="42">
+        <v>7108</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F10" s="42">
+        <v>129</v>
+      </c>
+      <c r="G10" s="62">
+        <f t="shared" si="0"/>
+        <v>791.41499999999996</v>
+      </c>
+      <c r="H10" s="56">
+        <f t="shared" si="1"/>
+        <v>141.255</v>
+      </c>
+      <c r="I10" s="62">
+        <f t="shared" si="2"/>
+        <v>866.599425</v>
+      </c>
+      <c r="J10" s="81">
+        <f t="shared" si="4"/>
+        <v>1004.5893387499999</v>
+      </c>
+      <c r="K10" s="102">
+        <v>1009</v>
+      </c>
+      <c r="L10" s="110">
+        <f t="shared" si="3"/>
+        <v>142.400575</v>
+      </c>
+      <c r="N10" s="100"/>
+      <c r="O10" s="99">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P10" s="106"/>
+    </row>
+    <row r="11" spans="2:16" ht="22" customHeight="1">
+      <c r="B11" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="C11" s="40">
+        <v>7109</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F11" s="42">
+        <v>129</v>
+      </c>
+      <c r="G11" s="62">
+        <f t="shared" si="0"/>
+        <v>791.41499999999996</v>
+      </c>
+      <c r="H11" s="56">
+        <f t="shared" si="1"/>
+        <v>141.255</v>
+      </c>
+      <c r="I11" s="62">
+        <f t="shared" si="2"/>
+        <v>866.599425</v>
+      </c>
+      <c r="J11" s="81">
+        <f t="shared" si="4"/>
+        <v>1004.5893387499999</v>
+      </c>
+      <c r="K11" s="102">
+        <v>1009</v>
+      </c>
+      <c r="L11" s="110">
+        <f t="shared" si="3"/>
+        <v>142.400575</v>
+      </c>
+      <c r="N11" s="42"/>
+      <c r="O11" s="99">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P11" s="106"/>
+    </row>
+    <row r="12" spans="2:16" ht="22" customHeight="1">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="110"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="99"/>
+      <c r="P12" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the discount for Clinique
</commit_message>
<xml_diff>
--- a/Logpie.xlsx
+++ b/Logpie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="护肤品1000" sheetId="1" r:id="rId1"/>
@@ -1512,8 +1512,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
     <numFmt numFmtId="176" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -1898,7 +1899,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2309,6 +2310,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -2743,10 +2747,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0"/>
@@ -4807,12 +4811,17 @@
       <c r="O38" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="P38" s="11"/>
+      <c r="P38" s="141">
+        <f>F38*0.8</f>
+        <v>13.600000000000001</v>
+      </c>
       <c r="Q38" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R38" s="113"/>
+        <v>107.96000000000001</v>
+      </c>
+      <c r="R38" s="113">
+        <v>109</v>
+      </c>
       <c r="S38" s="14"/>
     </row>
     <row r="39" spans="2:19" ht="22" customHeight="1">
@@ -4861,12 +4870,17 @@
       <c r="O39" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="P39" s="11"/>
+      <c r="P39" s="141">
+        <f t="shared" ref="P39:P43" si="18">F39*0.8</f>
+        <v>11.200000000000001</v>
+      </c>
       <c r="Q39" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R39" s="113"/>
+        <v>90.320000000000007</v>
+      </c>
+      <c r="R39" s="113">
+        <v>89</v>
+      </c>
       <c r="S39" s="14"/>
     </row>
     <row r="40" spans="2:19" ht="22" customHeight="1">
@@ -4913,12 +4927,17 @@
       <c r="O40" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="P40" s="11"/>
+      <c r="P40" s="141">
+        <f t="shared" si="18"/>
+        <v>11.600000000000001</v>
+      </c>
       <c r="Q40" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R40" s="113"/>
+        <v>93.26</v>
+      </c>
+      <c r="R40" s="113">
+        <v>95</v>
+      </c>
       <c r="S40" s="14"/>
     </row>
     <row r="41" spans="2:19" ht="22" customHeight="1">
@@ -4967,12 +4986,17 @@
       <c r="O41" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="P41" s="11"/>
+      <c r="P41" s="141">
+        <f t="shared" si="18"/>
+        <v>20.8</v>
+      </c>
       <c r="Q41" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R41" s="113"/>
+        <v>160.88</v>
+      </c>
+      <c r="R41" s="113">
+        <v>159</v>
+      </c>
       <c r="S41" s="14"/>
     </row>
     <row r="42" spans="2:19" ht="22" customHeight="1">
@@ -5019,12 +5043,17 @@
       <c r="O42" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="P42" s="11"/>
+      <c r="P42" s="141">
+        <f t="shared" si="18"/>
+        <v>11.600000000000001</v>
+      </c>
       <c r="Q42" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R42" s="113"/>
+        <v>93.26</v>
+      </c>
+      <c r="R42" s="113">
+        <v>95</v>
+      </c>
       <c r="S42" s="14"/>
     </row>
     <row r="43" spans="2:19" ht="22" customHeight="1">
@@ -5073,12 +5102,17 @@
       <c r="O43" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="P43" s="11"/>
+      <c r="P43" s="141">
+        <f t="shared" si="18"/>
+        <v>20.8</v>
+      </c>
       <c r="Q43" s="11">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R43" s="113"/>
+        <v>160.88</v>
+      </c>
+      <c r="R43" s="113">
+        <v>159</v>
+      </c>
       <c r="S43" s="14"/>
     </row>
     <row r="44" spans="2:19" ht="22" customHeight="1">
@@ -5121,15 +5155,15 @@
         <v>25</v>
       </c>
       <c r="G45" s="13">
-        <f t="shared" ref="G45:G50" si="18">F45*6.135</f>
+        <f t="shared" ref="G45:G50" si="19">F45*6.135</f>
         <v>153.375</v>
       </c>
       <c r="H45" s="12">
-        <f t="shared" ref="H45:H50" si="19">F45*(1+0.095)</f>
+        <f t="shared" ref="H45:H50" si="20">F45*(1+0.095)</f>
         <v>27.375</v>
       </c>
       <c r="I45" s="13">
-        <f t="shared" ref="I45:I50" si="20">H45*6.135</f>
+        <f t="shared" ref="I45:I50" si="21">H45*6.135</f>
         <v>167.94562500000001</v>
       </c>
       <c r="J45" s="81">
@@ -5140,7 +5174,7 @@
         <v>229</v>
       </c>
       <c r="L45" s="78">
-        <f t="shared" ref="L45:L50" si="21">K45-I45</f>
+        <f t="shared" ref="L45:L50" si="22">K45-I45</f>
         <v>61.054374999999993</v>
       </c>
       <c r="M45" s="136" t="s">
@@ -5175,15 +5209,15 @@
         <v>36</v>
       </c>
       <c r="G46" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>220.85999999999999</v>
       </c>
       <c r="H46" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>39.42</v>
       </c>
       <c r="I46" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>241.8417</v>
       </c>
       <c r="J46" s="81">
@@ -5194,7 +5228,7 @@
         <v>279</v>
       </c>
       <c r="L46" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>37.158299999999997</v>
       </c>
       <c r="M46" s="137"/>
@@ -5225,15 +5259,15 @@
         <v>43</v>
       </c>
       <c r="G47" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>263.80500000000001</v>
       </c>
       <c r="H47" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>47.085000000000001</v>
       </c>
       <c r="I47" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>288.86647499999998</v>
       </c>
       <c r="J47" s="81">
@@ -5244,7 +5278,7 @@
         <v>329</v>
       </c>
       <c r="L47" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>40.13352500000002</v>
       </c>
       <c r="M47" s="137"/>
@@ -5279,15 +5313,15 @@
         <v>65</v>
       </c>
       <c r="G48" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>398.77499999999998</v>
       </c>
       <c r="H48" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>71.174999999999997</v>
       </c>
       <c r="I48" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>436.65862499999997</v>
       </c>
       <c r="J48" s="81">
@@ -5298,7 +5332,7 @@
         <v>479</v>
       </c>
       <c r="L48" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>42.341375000000028</v>
       </c>
       <c r="M48" s="137"/>
@@ -5333,15 +5367,15 @@
         <v>84</v>
       </c>
       <c r="G49" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>515.34</v>
       </c>
       <c r="H49" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>91.98</v>
       </c>
       <c r="I49" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>564.29729999999995</v>
       </c>
       <c r="J49" s="81">
@@ -5352,7 +5386,7 @@
         <v>639</v>
       </c>
       <c r="L49" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>74.70270000000005</v>
       </c>
       <c r="M49" s="137"/>
@@ -5385,15 +5419,15 @@
         <v>104</v>
       </c>
       <c r="G50" s="13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>638.04</v>
       </c>
       <c r="H50" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>113.88</v>
       </c>
       <c r="I50" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>698.65379999999993</v>
       </c>
       <c r="J50" s="81">
@@ -5404,7 +5438,7 @@
         <v>769</v>
       </c>
       <c r="L50" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>70.346200000000067</v>
       </c>
       <c r="M50" s="137"/>
@@ -5546,7 +5580,7 @@
         <v>143</v>
       </c>
       <c r="P53" s="12">
-        <f t="shared" ref="P53:P55" si="22">H53*0.8</f>
+        <f t="shared" ref="P53:P55" si="23">H53*0.8</f>
         <v>20.148</v>
       </c>
       <c r="Q53" s="11">
@@ -5603,7 +5637,7 @@
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>26.28</v>
       </c>
       <c r="Q54" s="11">
@@ -5662,7 +5696,7 @@
         <v>144</v>
       </c>
       <c r="P55" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>36.792000000000002</v>
       </c>
       <c r="Q55" s="11">
@@ -5711,15 +5745,15 @@
         <v>25</v>
       </c>
       <c r="G57" s="13">
-        <f t="shared" ref="G57:G63" si="23">F57*6.135</f>
+        <f t="shared" ref="G57:G63" si="24">F57*6.135</f>
         <v>153.375</v>
       </c>
       <c r="H57" s="12">
-        <f t="shared" ref="H57:H63" si="24">F57*(1+0.095)</f>
+        <f t="shared" ref="H57:H63" si="25">F57*(1+0.095)</f>
         <v>27.375</v>
       </c>
       <c r="I57" s="13">
-        <f t="shared" ref="I57:I63" si="25">H57*6.135</f>
+        <f t="shared" ref="I57:I63" si="26">H57*6.135</f>
         <v>167.94562500000001</v>
       </c>
       <c r="J57" s="81">
@@ -5730,7 +5764,7 @@
         <v>209</v>
       </c>
       <c r="L57" s="78">
-        <f t="shared" ref="L57:L68" si="26">K57-I57</f>
+        <f t="shared" ref="L57:L68" si="27">K57-I57</f>
         <v>41.054374999999993</v>
       </c>
       <c r="M57" s="11"/>
@@ -5765,15 +5799,15 @@
         <v>25</v>
       </c>
       <c r="G58" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>153.375</v>
       </c>
       <c r="H58" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>27.375</v>
       </c>
       <c r="I58" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>167.94562500000001</v>
       </c>
       <c r="J58" s="81">
@@ -5784,7 +5818,7 @@
         <v>209</v>
       </c>
       <c r="L58" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>41.054374999999993</v>
       </c>
       <c r="M58" s="11"/>
@@ -5819,15 +5853,15 @@
         <v>25</v>
       </c>
       <c r="G59" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>153.375</v>
       </c>
       <c r="H59" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>27.375</v>
       </c>
       <c r="I59" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>167.94562500000001</v>
       </c>
       <c r="J59" s="81">
@@ -5838,7 +5872,7 @@
         <v>209</v>
       </c>
       <c r="L59" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>41.054374999999993</v>
       </c>
       <c r="M59" s="11"/>
@@ -5873,15 +5907,15 @@
         <v>31</v>
       </c>
       <c r="G60" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>190.185</v>
       </c>
       <c r="H60" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>33.945</v>
       </c>
       <c r="I60" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>208.25257500000001</v>
       </c>
       <c r="J60" s="81">
@@ -5892,7 +5926,7 @@
         <v>249</v>
       </c>
       <c r="L60" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>40.747424999999993</v>
       </c>
       <c r="M60" s="11"/>
@@ -5927,15 +5961,15 @@
         <v>41</v>
       </c>
       <c r="G61" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>251.535</v>
       </c>
       <c r="H61" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>44.894999999999996</v>
       </c>
       <c r="I61" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>275.43082499999997</v>
       </c>
       <c r="J61" s="81">
@@ -5946,7 +5980,7 @@
         <v>329</v>
       </c>
       <c r="L61" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>53.56917500000003</v>
       </c>
       <c r="M61" s="11"/>
@@ -5981,15 +6015,15 @@
         <v>41</v>
       </c>
       <c r="G62" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>251.535</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>44.894999999999996</v>
       </c>
       <c r="I62" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>275.43082499999997</v>
       </c>
       <c r="J62" s="81">
@@ -6000,7 +6034,7 @@
         <v>329</v>
       </c>
       <c r="L62" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>53.56917500000003</v>
       </c>
       <c r="M62" s="11"/>
@@ -6035,15 +6069,15 @@
         <v>53</v>
       </c>
       <c r="G63" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>162.57749999999999</v>
       </c>
       <c r="H63" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.017499999999998</v>
       </c>
       <c r="I63" s="13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>178.02236249999999</v>
       </c>
       <c r="J63" s="81">
@@ -6054,7 +6088,7 @@
         <v>219</v>
       </c>
       <c r="L63" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>40.977637500000014</v>
       </c>
       <c r="M63" s="11"/>
@@ -6087,7 +6121,7 @@
       </c>
       <c r="K64" s="9"/>
       <c r="L64" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M64" s="11"/>
@@ -6137,7 +6171,7 @@
         <v>539</v>
       </c>
       <c r="L65" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>75.470075000000065</v>
       </c>
       <c r="M65" s="133" t="s">
@@ -6193,7 +6227,7 @@
         <v>539</v>
       </c>
       <c r="L66" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>75.470075000000065</v>
       </c>
       <c r="M66" s="134"/>
@@ -6247,7 +6281,7 @@
         <v>539</v>
       </c>
       <c r="L67" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>75.470075000000065</v>
       </c>
       <c r="M67" s="134"/>
@@ -6294,14 +6328,14 @@
         <v>463.52992499999993</v>
       </c>
       <c r="J68" s="81">
-        <f t="shared" ref="J68" si="27">I68*1.15+8</f>
+        <f t="shared" ref="J68" si="28">I68*1.15+8</f>
         <v>541.05941374999986</v>
       </c>
       <c r="K68" s="85">
         <v>539</v>
       </c>
       <c r="L68" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>75.470075000000065</v>
       </c>
       <c r="M68" s="134"/>
@@ -6313,7 +6347,7 @@
       </c>
       <c r="P68" s="11"/>
       <c r="Q68" s="11">
-        <f t="shared" ref="Q68" si="28">P68*6.125*1.2+8</f>
+        <f t="shared" ref="Q68" si="29">P68*6.125*1.2+8</f>
         <v>8</v>
       </c>
       <c r="R68" s="113"/>
@@ -13067,7 +13101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -13627,21 +13661,21 @@
         <v>1343.5650000000001</v>
       </c>
       <c r="J13" s="81">
-        <f>I13*1.15+8</f>
+        <f t="shared" ref="J13:J21" si="9">I13*1.15+8</f>
         <v>1553.0997499999999</v>
       </c>
       <c r="K13" s="101">
         <v>1559</v>
       </c>
       <c r="L13" s="110">
-        <f t="shared" ref="L13" si="9">K13-I13</f>
+        <f t="shared" ref="L13" si="10">K13-I13</f>
         <v>215.43499999999995</v>
       </c>
       <c r="N13" s="98">
         <v>59</v>
       </c>
       <c r="O13" s="99">
-        <f>N13*6.125*1.2+8</f>
+        <f t="shared" ref="O13:O21" si="11">N13*6.125*1.2+8</f>
         <v>441.65</v>
       </c>
       <c r="P13" s="105">
@@ -13677,7 +13711,7 @@
         <v>1645.8671249999998</v>
       </c>
       <c r="J14" s="81">
-        <f>I14*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1900.7471937499995</v>
       </c>
       <c r="K14" s="101">
@@ -13691,7 +13725,7 @@
         <v>59</v>
       </c>
       <c r="O14" s="99">
-        <f>N14*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P14" s="105">
@@ -13727,7 +13761,7 @@
         <v>1645.8671249999998</v>
       </c>
       <c r="J15" s="81">
-        <f>I15*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1900.7471937499995</v>
       </c>
       <c r="K15" s="101">
@@ -13741,7 +13775,7 @@
         <v>59</v>
       </c>
       <c r="O15" s="99">
-        <f>N15*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P15" s="105">
@@ -13765,33 +13799,33 @@
         <v>160</v>
       </c>
       <c r="G16" s="66">
-        <f t="shared" ref="G16:G21" si="10">F16*6.135</f>
+        <f t="shared" ref="G16:G21" si="12">F16*6.135</f>
         <v>981.59999999999991</v>
       </c>
       <c r="H16" s="60">
-        <f t="shared" ref="H16:H21" si="11">F16*(1+0.095)</f>
+        <f t="shared" ref="H16:H21" si="13">F16*(1+0.095)</f>
         <v>175.2</v>
       </c>
       <c r="I16" s="66">
-        <f t="shared" ref="I16:I21" si="12">H16*6.135</f>
+        <f t="shared" ref="I16:I21" si="14">H16*6.135</f>
         <v>1074.8519999999999</v>
       </c>
       <c r="J16" s="81">
-        <f>I16*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1244.0797999999998</v>
       </c>
       <c r="K16" s="101">
         <v>1259</v>
       </c>
       <c r="L16" s="110">
-        <f t="shared" ref="L16:L21" si="13">K16-I16</f>
+        <f t="shared" ref="L16:L21" si="15">K16-I16</f>
         <v>184.14800000000014</v>
       </c>
       <c r="N16" s="98">
         <v>59</v>
       </c>
       <c r="O16" s="99">
-        <f>N16*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P16" s="105">
@@ -13815,33 +13849,33 @@
         <v>205</v>
       </c>
       <c r="G17" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1257.675</v>
       </c>
       <c r="H17" s="60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>224.47499999999999</v>
       </c>
       <c r="I17" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1377.154125</v>
       </c>
       <c r="J17" s="81">
-        <f>I17*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1591.7272437499998</v>
       </c>
       <c r="K17" s="101">
         <v>1599</v>
       </c>
       <c r="L17" s="110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>221.84587499999998</v>
       </c>
       <c r="N17" s="98">
         <v>59</v>
       </c>
       <c r="O17" s="99">
-        <f>N17*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P17" s="105">
@@ -13865,33 +13899,33 @@
         <v>170</v>
       </c>
       <c r="G18" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1042.95</v>
       </c>
       <c r="H18" s="60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>186.15</v>
       </c>
       <c r="I18" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1142.03025</v>
       </c>
       <c r="J18" s="81">
-        <f>I18*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1321.3347874999999</v>
       </c>
       <c r="K18" s="101">
         <v>1359</v>
       </c>
       <c r="L18" s="110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>216.96974999999998</v>
       </c>
       <c r="N18" s="98">
         <v>59</v>
       </c>
       <c r="O18" s="99">
-        <f>N18*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P18" s="105">
@@ -13915,33 +13949,33 @@
         <v>170</v>
       </c>
       <c r="G19" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1042.95</v>
       </c>
       <c r="H19" s="60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>186.15</v>
       </c>
       <c r="I19" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1142.03025</v>
       </c>
       <c r="J19" s="81">
-        <f>I19*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>1321.3347874999999</v>
       </c>
       <c r="K19" s="101">
         <v>1359</v>
       </c>
       <c r="L19" s="110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>216.96974999999998</v>
       </c>
       <c r="N19" s="98">
         <v>59</v>
       </c>
       <c r="O19" s="99">
-        <f>N19*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P19" s="105">
@@ -13961,33 +13995,33 @@
       </c>
       <c r="F20" s="40"/>
       <c r="G20" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H20" s="60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I20" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J20" s="81">
-        <f>I20*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="K20" s="101">
         <v>619</v>
       </c>
       <c r="L20" s="110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>619</v>
       </c>
       <c r="N20" s="98">
         <v>59</v>
       </c>
       <c r="O20" s="99">
-        <f>N20*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P20" s="105">
@@ -14007,33 +14041,33 @@
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H21" s="60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I21" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J21" s="81">
-        <f>I21*1.15+8</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="K21" s="101">
         <v>619</v>
       </c>
       <c r="L21" s="110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>619</v>
       </c>
       <c r="N21" s="98">
         <v>59</v>
       </c>
       <c r="O21" s="99">
-        <f>N21*6.125*1.2+8</f>
+        <f t="shared" si="11"/>
         <v>441.65</v>
       </c>
       <c r="P21" s="105">

</xml_diff>